<commit_message>
Added bearroot and avoid copying settings file during tests
</commit_message>
<xml_diff>
--- a/tbx/bear/data.xlsx
+++ b/tbx/bear/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7785" tabRatio="946" firstSheet="15" activeTab="25"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7785" tabRatio="946" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="12" r:id="rId1"/>
@@ -44,6 +44,9 @@
     <sheet name="pan blocks" sheetId="47" r:id="rId35"/>
     <sheet name="DSAFO32ADVVERINF32" sheetId="50" state="hidden" r:id="rId36"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId37"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_DLX1.INC" localSheetId="12">#REF!</definedName>
     <definedName name="_DLX1.INC" localSheetId="13">#REF!</definedName>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="1611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="1613">
   <si>
     <t>1999q1</t>
   </si>
@@ -5014,9 +5017,6 @@
     <t>AR prior</t>
   </si>
   <si>
-    <t>0 0.1</t>
-  </si>
-  <si>
     <t>Exogenous variables - tightness</t>
   </si>
   <si>
@@ -5038,9 +5038,6 @@
     <t>Constant</t>
   </si>
   <si>
-    <t>2003q2 2014q4</t>
-  </si>
-  <si>
     <t>transformation</t>
   </si>
   <si>
@@ -5065,6 +5062,12 @@
     <t>S1</t>
   </si>
   <si>
+    <t>Weaker</t>
+  </si>
+  <si>
+    <t>Stronger</t>
+  </si>
+  <si>
     <t>.Absolute</t>
   </si>
   <si>
@@ -5074,10 +5077,16 @@
     <t xml:space="preserve">&gt;50% </t>
   </si>
   <si>
-    <t>Weaker.W1</t>
-  </si>
-  <si>
-    <t>Stronger.S1</t>
+    <t>9 10</t>
+  </si>
+  <si>
+    <t>2008q2 2014q4</t>
+  </si>
+  <si>
+    <t>0 2</t>
+  </si>
+  <si>
+    <t>0 3</t>
   </si>
 </sst>
 </file>
@@ -5101,7 +5110,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -6243,7 +6251,7 @@
     <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6479,6 +6487,9 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6612,6 +6623,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="data"/>
+      <sheetName val="US"/>
+      <sheetName val="EA"/>
+      <sheetName val="UK"/>
+      <sheetName val="yearly"/>
+      <sheetName val="quarterly"/>
+      <sheetName val="monthly"/>
+      <sheetName val="weekly"/>
+      <sheetName val="daily"/>
+      <sheetName val="undated"/>
+      <sheetName val="AR priors"/>
+      <sheetName val="exo mean priors"/>
+      <sheetName val="exo tight priors"/>
+      <sheetName val="mean adj prior"/>
+      <sheetName val="Long run prior"/>
+      <sheetName val="pred exo"/>
+      <sheetName val="grid"/>
+      <sheetName val="block exo"/>
+      <sheetName val="sign res values"/>
+      <sheetName val="sign res periods"/>
+      <sheetName val="conditions"/>
+      <sheetName val="shocks"/>
+      <sheetName val="blocks"/>
+      <sheetName val="intervals"/>
+      <sheetName val="pan pred exo"/>
+      <sheetName val="pan conditions"/>
+      <sheetName val="pan shocks"/>
+      <sheetName val="pan blocks"/>
+      <sheetName val="DSAFO32ADVVERINF32"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>DOM_GDP</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>Constant</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6906,8 +6998,8 @@
   </sheetPr>
   <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7398,7 +7490,7 @@
       </c>
       <c r="G27" s="63"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>1382</v>
       </c>
@@ -7416,7 +7508,7 @@
       </c>
       <c r="G28" s="63"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>1383</v>
       </c>
@@ -7434,7 +7526,7 @@
       </c>
       <c r="G29" s="63"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
         <v>1384</v>
       </c>
@@ -7452,7 +7544,7 @@
       </c>
       <c r="G30" s="63"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
         <v>1385</v>
       </c>
@@ -7470,7 +7562,7 @@
       </c>
       <c r="G31" s="63"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="43" t="s">
         <v>1386</v>
       </c>
@@ -7488,7 +7580,7 @@
       </c>
       <c r="G32" s="63"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="43" t="s">
         <v>1387</v>
       </c>
@@ -7506,7 +7598,7 @@
       </c>
       <c r="G33" s="63"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="43" t="s">
         <v>1388</v>
       </c>
@@ -7524,7 +7616,7 @@
       </c>
       <c r="G34" s="63"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="43" t="s">
         <v>1389</v>
       </c>
@@ -7542,7 +7634,7 @@
       </c>
       <c r="G35" s="63"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>1390</v>
       </c>
@@ -7560,7 +7652,7 @@
       </c>
       <c r="G36" s="63"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
         <v>1391</v>
       </c>
@@ -7578,7 +7670,7 @@
       </c>
       <c r="G37" s="63"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
         <v>1392</v>
       </c>
@@ -7596,7 +7688,7 @@
       </c>
       <c r="G38" s="63"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>1393</v>
       </c>
@@ -7614,7 +7706,7 @@
       </c>
       <c r="G39" s="63"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
         <v>1394</v>
       </c>
@@ -7632,7 +7724,7 @@
       </c>
       <c r="G40" s="63"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>1395</v>
       </c>
@@ -7650,7 +7742,7 @@
       </c>
       <c r="G41" s="63"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>1396</v>
       </c>
@@ -7668,7 +7760,7 @@
       </c>
       <c r="G42" s="63"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
         <v>1397</v>
       </c>
@@ -7686,7 +7778,7 @@
       </c>
       <c r="G43" s="63"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
         <v>1398</v>
       </c>
@@ -7704,7 +7796,7 @@
       </c>
       <c r="G44" s="63"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
         <v>1399</v>
       </c>
@@ -7722,7 +7814,7 @@
       </c>
       <c r="G45" s="63"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="44" t="s">
         <v>1400</v>
       </c>
@@ -7740,7 +7832,7 @@
       </c>
       <c r="G46" s="63"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="44" t="s">
         <v>1401</v>
       </c>
@@ -7758,7 +7850,7 @@
       </c>
       <c r="G47" s="63"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="44" t="s">
         <v>1402</v>
       </c>
@@ -7776,7 +7868,7 @@
       </c>
       <c r="G48" s="63"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="44" t="s">
         <v>1403</v>
       </c>
@@ -7794,7 +7886,7 @@
       </c>
       <c r="G49" s="63"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="44" t="s">
         <v>1404</v>
       </c>
@@ -7812,7 +7904,7 @@
       </c>
       <c r="G50" s="63"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
         <v>1405</v>
       </c>
@@ -7830,7 +7922,7 @@
       </c>
       <c r="G51" s="63"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="44" t="s">
         <v>1406</v>
       </c>
@@ -7848,7 +7940,7 @@
       </c>
       <c r="G52" s="63"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="44" t="s">
         <v>1407</v>
       </c>
@@ -7866,7 +7958,7 @@
       </c>
       <c r="G53" s="63"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="44" t="s">
         <v>1408</v>
       </c>
@@ -7884,7 +7976,7 @@
       </c>
       <c r="G54" s="63"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="44" t="s">
         <v>1409</v>
       </c>
@@ -7902,7 +7994,7 @@
       </c>
       <c r="G55" s="63"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="44" t="s">
         <v>1410</v>
       </c>
@@ -7920,7 +8012,7 @@
       </c>
       <c r="G56" s="63"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="44" t="s">
         <v>1411</v>
       </c>
@@ -7938,7 +8030,7 @@
       </c>
       <c r="G57" s="63"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="44" t="s">
         <v>1412</v>
       </c>
@@ -7956,7 +8048,7 @@
       </c>
       <c r="G58" s="63"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="44" t="s">
         <v>1413</v>
       </c>
@@ -7974,7 +8066,7 @@
       </c>
       <c r="G59" s="63"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="44" t="s">
         <v>1414</v>
       </c>
@@ -7992,7 +8084,7 @@
       </c>
       <c r="G60" s="63"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="44" t="s">
         <v>1415</v>
       </c>
@@ -8010,7 +8102,7 @@
       </c>
       <c r="G61" s="63"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="44" t="s">
         <v>1416</v>
       </c>
@@ -8028,7 +8120,7 @@
       </c>
       <c r="G62" s="63"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="44" t="s">
         <v>1417</v>
       </c>
@@ -8046,7 +8138,7 @@
       </c>
       <c r="G63" s="63"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="44" t="s">
         <v>1418</v>
       </c>
@@ -8064,7 +8156,7 @@
       </c>
       <c r="G64" s="63"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="44" t="s">
         <v>1419</v>
       </c>
@@ -8082,7 +8174,7 @@
       </c>
       <c r="G65" s="63"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="44" t="s">
         <v>1420</v>
       </c>
@@ -8100,7 +8192,7 @@
       </c>
       <c r="G66" s="63"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="44" t="s">
         <v>1421</v>
       </c>
@@ -8118,7 +8210,7 @@
       </c>
       <c r="G67" s="63"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="44" t="s">
         <v>1422</v>
       </c>
@@ -8136,7 +8228,7 @@
       </c>
       <c r="G68" s="63"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="44" t="s">
         <v>1423</v>
       </c>
@@ -8154,7 +8246,7 @@
       </c>
       <c r="G69" s="63"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="44" t="s">
         <v>1424</v>
       </c>
@@ -8172,7 +8264,7 @@
       </c>
       <c r="G70" s="63"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="44" t="s">
         <v>1425</v>
       </c>
@@ -8190,7 +8282,7 @@
       </c>
       <c r="G71" s="63"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="44" t="s">
         <v>1426</v>
       </c>
@@ -8208,7 +8300,7 @@
       </c>
       <c r="G72" s="63"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="44" t="s">
         <v>1427</v>
       </c>
@@ -8226,7 +8318,7 @@
       </c>
       <c r="G73" s="63"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="44" t="s">
         <v>1428</v>
       </c>
@@ -8244,7 +8336,7 @@
       </c>
       <c r="G74" s="63"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="44" t="s">
         <v>1429</v>
       </c>
@@ -8262,7 +8354,7 @@
       </c>
       <c r="G75" s="63"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="44" t="s">
         <v>1430</v>
       </c>
@@ -8280,7 +8372,7 @@
       </c>
       <c r="G76" s="63"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="44" t="s">
         <v>1431</v>
       </c>
@@ -8298,7 +8390,7 @@
       </c>
       <c r="G77" s="63"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="44" t="s">
         <v>1432</v>
       </c>
@@ -8316,7 +8408,7 @@
       </c>
       <c r="G78" s="63"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="44" t="s">
         <v>1433</v>
       </c>
@@ -8334,7 +8426,7 @@
       </c>
       <c r="G79" s="63"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="44" t="s">
         <v>1434</v>
       </c>
@@ -8352,7 +8444,7 @@
       </c>
       <c r="G80" s="63"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="44" t="s">
         <v>1435</v>
       </c>
@@ -8370,7 +8462,7 @@
       </c>
       <c r="G81" s="63"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="44" t="s">
         <v>1436</v>
       </c>
@@ -8388,7 +8480,7 @@
       </c>
       <c r="G82" s="63"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="44" t="s">
         <v>1437</v>
       </c>
@@ -8406,7 +8498,7 @@
       </c>
       <c r="G83" s="63"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="44" t="s">
         <v>1438</v>
       </c>
@@ -8424,7 +8516,7 @@
       </c>
       <c r="G84" s="63"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="44" t="s">
         <v>1439</v>
       </c>
@@ -8442,7 +8534,7 @@
       </c>
       <c r="G85" s="63"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="44" t="s">
         <v>1440</v>
       </c>
@@ -8460,7 +8552,7 @@
       </c>
       <c r="G86" s="63"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="44" t="s">
         <v>1441</v>
       </c>
@@ -8478,7 +8570,7 @@
       </c>
       <c r="G87" s="63"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="44" t="s">
         <v>1442</v>
       </c>
@@ -8496,7 +8588,7 @@
       </c>
       <c r="G88" s="63"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="44" t="s">
         <v>1443</v>
       </c>
@@ -8514,7 +8606,7 @@
       </c>
       <c r="G89" s="63"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90" s="44" t="s">
         <v>1444</v>
       </c>
@@ -8532,7 +8624,7 @@
       </c>
       <c r="G90" s="63"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="44" t="s">
         <v>1445</v>
       </c>
@@ -8550,7 +8642,7 @@
       </c>
       <c r="G91" s="63"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="44" t="s">
         <v>1334</v>
       </c>
@@ -8568,7 +8660,7 @@
       </c>
       <c r="G92" s="63"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="44" t="s">
         <v>1335</v>
       </c>
@@ -8586,7 +8678,7 @@
       </c>
       <c r="G93" s="63"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="44" t="s">
         <v>1336</v>
       </c>
@@ -8604,7 +8696,7 @@
       </c>
       <c r="G94" s="63"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="44" t="s">
         <v>1337</v>
       </c>
@@ -8622,7 +8714,7 @@
       </c>
       <c r="G95" s="63"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96" s="44" t="s">
         <v>1338</v>
       </c>
@@ -8640,7 +8732,7 @@
       </c>
       <c r="G96" s="63"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="44" t="s">
         <v>1339</v>
       </c>
@@ -8658,7 +8750,7 @@
       </c>
       <c r="G97" s="63"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98" s="44" t="s">
         <v>1340</v>
       </c>
@@ -8676,7 +8768,7 @@
       </c>
       <c r="G98" s="63"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="44" t="s">
         <v>1341</v>
       </c>
@@ -8694,7 +8786,7 @@
       </c>
       <c r="G99" s="63"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
         <v>1342</v>
       </c>
@@ -8712,7 +8804,7 @@
       </c>
       <c r="G100" s="63"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
         <v>1343</v>
       </c>
@@ -8730,7 +8822,7 @@
       </c>
       <c r="G101" s="63"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
         <v>0</v>
       </c>
@@ -8748,7 +8840,7 @@
       </c>
       <c r="G102" s="63"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
         <v>1</v>
       </c>
@@ -8766,7 +8858,7 @@
       </c>
       <c r="G103" s="63"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
         <v>2</v>
       </c>
@@ -8784,7 +8876,7 @@
       </c>
       <c r="G104" s="63"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105" s="44" t="s">
         <v>3</v>
       </c>
@@ -8802,7 +8894,7 @@
       </c>
       <c r="G105" s="63"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
         <v>4</v>
       </c>
@@ -8820,7 +8912,7 @@
       </c>
       <c r="G106" s="63"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107" s="44" t="s">
         <v>5</v>
       </c>
@@ -8838,7 +8930,7 @@
       </c>
       <c r="G107" s="63"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="44" t="s">
         <v>6</v>
       </c>
@@ -8856,7 +8948,7 @@
       </c>
       <c r="G108" s="63"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A109" s="44" t="s">
         <v>7</v>
       </c>
@@ -8874,7 +8966,7 @@
       </c>
       <c r="G109" s="63"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="44" t="s">
         <v>8</v>
       </c>
@@ -8892,7 +8984,7 @@
       </c>
       <c r="G110" s="63"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="44" t="s">
         <v>9</v>
       </c>
@@ -8910,7 +9002,7 @@
       </c>
       <c r="G111" s="63"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="44" t="s">
         <v>10</v>
       </c>
@@ -8928,7 +9020,7 @@
       </c>
       <c r="G112" s="63"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="44" t="s">
         <v>11</v>
       </c>
@@ -8946,7 +9038,7 @@
       </c>
       <c r="G113" s="63"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
         <v>12</v>
       </c>
@@ -8964,7 +9056,7 @@
       </c>
       <c r="G114" s="63"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="44" t="s">
         <v>13</v>
       </c>
@@ -8982,7 +9074,7 @@
       </c>
       <c r="G115" s="63"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>14</v>
       </c>
@@ -9000,7 +9092,7 @@
       </c>
       <c r="G116" s="63"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="44" t="s">
         <v>15</v>
       </c>
@@ -9018,7 +9110,7 @@
       </c>
       <c r="G117" s="63"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
         <v>16</v>
       </c>
@@ -9036,7 +9128,7 @@
       </c>
       <c r="G118" s="63"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="44" t="s">
         <v>17</v>
       </c>
@@ -9054,7 +9146,7 @@
       </c>
       <c r="G119" s="63"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="44" t="s">
         <v>18</v>
       </c>
@@ -9072,7 +9164,7 @@
       </c>
       <c r="G120" s="63"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="44" t="s">
         <v>19</v>
       </c>
@@ -9090,7 +9182,7 @@
       </c>
       <c r="G121" s="63"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="44" t="s">
         <v>20</v>
       </c>
@@ -9108,7 +9200,7 @@
       </c>
       <c r="G122" s="63"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="44" t="s">
         <v>21</v>
       </c>
@@ -9126,7 +9218,7 @@
       </c>
       <c r="G123" s="63"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="44" t="s">
         <v>22</v>
       </c>
@@ -9144,7 +9236,7 @@
       </c>
       <c r="G124" s="63"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="44" t="s">
         <v>23</v>
       </c>
@@ -9162,7 +9254,7 @@
       </c>
       <c r="G125" s="63"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="44" t="s">
         <v>24</v>
       </c>
@@ -9180,7 +9272,7 @@
       </c>
       <c r="G126" s="63"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127" s="44" t="s">
         <v>25</v>
       </c>
@@ -9198,7 +9290,7 @@
       </c>
       <c r="G127" s="63"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128" s="44" t="s">
         <v>26</v>
       </c>
@@ -9216,7 +9308,7 @@
       </c>
       <c r="G128" s="63"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="44" t="s">
         <v>27</v>
       </c>
@@ -9234,7 +9326,7 @@
       </c>
       <c r="G129" s="63"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130" s="44" t="s">
         <v>28</v>
       </c>
@@ -9252,7 +9344,7 @@
       </c>
       <c r="G130" s="63"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131" s="44" t="s">
         <v>29</v>
       </c>
@@ -9270,7 +9362,7 @@
       </c>
       <c r="G131" s="63"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132" s="44" t="s">
         <v>30</v>
       </c>
@@ -9288,7 +9380,7 @@
       </c>
       <c r="G132" s="63"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A133" s="44" t="s">
         <v>31</v>
       </c>
@@ -9306,7 +9398,7 @@
       </c>
       <c r="G133" s="63"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134" s="44" t="s">
         <v>32</v>
       </c>
@@ -9324,7 +9416,7 @@
       </c>
       <c r="G134" s="63"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135" s="44" t="s">
         <v>33</v>
       </c>
@@ -9342,7 +9434,7 @@
       </c>
       <c r="G135" s="63"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136" s="44" t="s">
         <v>34</v>
       </c>
@@ -9360,7 +9452,7 @@
       </c>
       <c r="G136" s="63"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A137" s="44" t="s">
         <v>35</v>
       </c>
@@ -9378,7 +9470,7 @@
       </c>
       <c r="G137" s="63"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A138" s="44" t="s">
         <v>36</v>
       </c>
@@ -9396,7 +9488,7 @@
       </c>
       <c r="G138" s="63"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A139" s="44" t="s">
         <v>37</v>
       </c>
@@ -9414,7 +9506,7 @@
       </c>
       <c r="G139" s="63"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A140" s="44" t="s">
         <v>38</v>
       </c>
@@ -9432,7 +9524,7 @@
       </c>
       <c r="G140" s="63"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141" s="44" t="s">
         <v>39</v>
       </c>
@@ -9450,7 +9542,7 @@
       </c>
       <c r="G141" s="63"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142" s="44" t="s">
         <v>40</v>
       </c>
@@ -9468,7 +9560,7 @@
       </c>
       <c r="G142" s="63"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A143" s="44" t="s">
         <v>41</v>
       </c>
@@ -9486,7 +9578,7 @@
       </c>
       <c r="G143" s="63"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A144" s="44" t="s">
         <v>42</v>
       </c>
@@ -9504,7 +9596,7 @@
       </c>
       <c r="G144" s="63"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A145" s="44" t="s">
         <v>43</v>
       </c>
@@ -9522,7 +9614,7 @@
       </c>
       <c r="G145" s="63"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A146" s="44" t="s">
         <v>44</v>
       </c>
@@ -9540,7 +9632,7 @@
       </c>
       <c r="G146" s="63"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A147" s="44" t="s">
         <v>45</v>
       </c>
@@ -9558,7 +9650,7 @@
       </c>
       <c r="G147" s="63"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A148" s="44" t="s">
         <v>46</v>
       </c>
@@ -9576,7 +9668,7 @@
       </c>
       <c r="G148" s="63"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="44" t="s">
         <v>47</v>
       </c>
@@ -9594,7 +9686,7 @@
       </c>
       <c r="G149" s="63"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="44" t="s">
         <v>48</v>
       </c>
@@ -9612,7 +9704,7 @@
       </c>
       <c r="G150" s="63"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="44" t="s">
         <v>49</v>
       </c>
@@ -9630,7 +9722,7 @@
       </c>
       <c r="G151" s="63"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="44" t="s">
         <v>50</v>
       </c>
@@ -9648,7 +9740,7 @@
       </c>
       <c r="G152" s="63"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A153" s="44" t="s">
         <v>51</v>
       </c>
@@ -9666,7 +9758,7 @@
       </c>
       <c r="G153" s="63"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="44" t="s">
         <v>52</v>
       </c>
@@ -9684,7 +9776,7 @@
       </c>
       <c r="G154" s="63"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A155" s="44" t="s">
         <v>53</v>
       </c>
@@ -9702,7 +9794,7 @@
       </c>
       <c r="G155" s="63"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A156" s="44" t="s">
         <v>54</v>
       </c>
@@ -9720,7 +9812,7 @@
       </c>
       <c r="G156" s="63"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A157" s="44" t="s">
         <v>55</v>
       </c>
@@ -9738,7 +9830,7 @@
       </c>
       <c r="G157" s="63"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A158" s="44" t="s">
         <v>56</v>
       </c>
@@ -9756,7 +9848,7 @@
       </c>
       <c r="G158" s="63"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="44" t="s">
         <v>57</v>
       </c>
@@ -9774,7 +9866,7 @@
       </c>
       <c r="G159" s="63"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A160" s="44" t="s">
         <v>58</v>
       </c>
@@ -9792,7 +9884,7 @@
       </c>
       <c r="G160" s="63"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A161" s="44" t="s">
         <v>59</v>
       </c>
@@ -9810,7 +9902,7 @@
       </c>
       <c r="G161" s="63"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A162" s="44" t="s">
         <v>60</v>
       </c>
@@ -9828,7 +9920,7 @@
       </c>
       <c r="G162" s="63"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A163" s="44" t="s">
         <v>61</v>
       </c>
@@ -9846,7 +9938,7 @@
       </c>
       <c r="G163" s="63"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A164" s="44" t="s">
         <v>62</v>
       </c>
@@ -9864,7 +9956,7 @@
       </c>
       <c r="G164" s="63"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A165" s="44" t="s">
         <v>63</v>
       </c>
@@ -9882,44 +9974,44 @@
       </c>
       <c r="G165" s="63"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="44"/>
       <c r="E166" s="2"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="44"/>
       <c r="E167" s="2"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="44"/>
       <c r="E168" s="2"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="44"/>
       <c r="E169" s="2"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="44"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="44"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="44"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="44"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="44"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="44"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="44"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="44"/>
     </row>
   </sheetData>
@@ -12961,60 +13053,60 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
-        <v>1598</v>
+      <c r="A1" s="92" t="s">
+        <v>1596</v>
       </c>
       <c r="B1" s="88">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="D1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="E1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="92" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="92" t="s">
         <v>1599</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B3" s="88" t="s">
         <v>1600</v>
       </c>
-      <c r="C2" t="s">
-        <v>1603</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1603</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="91" t="s">
+      <c r="C3" t="s">
         <v>1601</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1603</v>
-      </c>
       <c r="D3" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="E3" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -13030,7 +13122,7 @@
         <v>1357</v>
       </c>
       <c r="B5" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -13038,7 +13130,7 @@
         <v>1358</v>
       </c>
       <c r="B6" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -13046,7 +13138,7 @@
         <v>1359</v>
       </c>
       <c r="B7" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -13862,7 +13954,7 @@
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13872,10 +13964,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
         <v>1586</v>
       </c>
-      <c r="C2" s="99"/>
+      <c r="C2" s="100"/>
     </row>
     <row r="3" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="75" t="s">
@@ -13936,13 +14028,13 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="100"/>
+      <c r="G2" s="74" t="s">
         <v>1594</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99"/>
-      <c r="G2" s="74" t="s">
-        <v>1595</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -13950,14 +14042,14 @@
         <v>1587</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="D3" s="87" t="s">
         <v>1451</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="74" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -13971,7 +14063,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14023,28 +14115,29 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="100"/>
+      <c r="G2" s="74" t="s">
         <v>1590</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99"/>
-      <c r="G2" s="74" t="s">
-        <v>1591</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="75" t="s">
         <v>1587</v>
       </c>
-      <c r="C3" s="84" t="s">
-        <v>1596</v>
+      <c r="C3" s="84" t="str">
+        <f>'[1]exo mean priors'!C3</f>
+        <v>Constant</v>
       </c>
       <c r="D3" s="85" t="s">
         <v>1451</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="74" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14058,7 +14151,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14099,8 +14192,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14128,55 +14221,55 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
         <v>1331</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>1328</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>1446</v>
+      <c r="C3" s="96" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>1609</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>1597</v>
+        <v>1610</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="42" t="s">
         <v>1332</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="96" t="s">
         <v>1328</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="96" t="s">
         <v>1446</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>1597</v>
+        <v>1610</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
         <v>1333</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="96" t="s">
         <v>1328</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="96" t="s">
         <v>1455</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>1597</v>
+        <v>1610</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>1589</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -14213,7 +14306,7 @@
   <dimension ref="A2:A165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15301,7 +15394,7 @@
   <dimension ref="B1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18765,7 +18858,7 @@
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18775,26 +18868,25 @@
     <col min="9" max="9" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="11" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1583</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>1584</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>1585</v>
-      </c>
+    <row r="1" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="11"/>
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11"/>
+    <row r="2" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1584</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>1585</v>
+      </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -18820,13 +18912,13 @@
       <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="96" t="s">
         <v>1456</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="97" t="s">
         <v>1456</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="96" t="s">
         <v>1456</v>
       </c>
       <c r="F4" s="37"/>
@@ -18838,13 +18930,13 @@
       <c r="B5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="96" t="s">
         <v>1456</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="96" t="s">
         <v>1461</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="96" t="s">
         <v>1456</v>
       </c>
       <c r="F5" s="37"/>
@@ -18856,11 +18948,11 @@
       <c r="B6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="96" t="s">
         <v>1456</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95" t="s">
+      <c r="D6" s="96"/>
+      <c r="E6" s="96" t="s">
         <v>1461</v>
       </c>
       <c r="F6" s="37"/>
@@ -18930,7 +19022,7 @@
   <dimension ref="C1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18941,32 +19033,28 @@
     <col min="10" max="10" width="95.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="11" t="s">
-        <v>1582</v>
-      </c>
-      <c r="D1" s="16" t="str">
-        <f>'sign res values'!C1</f>
-        <v>Demand</v>
-      </c>
-      <c r="E1" s="16" t="str">
-        <f>'sign res values'!D1</f>
-        <v xml:space="preserve">Supply </v>
-      </c>
-      <c r="F1" s="16" t="str">
-        <f>'sign res values'!E1</f>
-        <v>Money</v>
-      </c>
+    <row r="1" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="16"/>
       <c r="H1" s="1"/>
       <c r="I1" s="11"/>
       <c r="J1" s="14"/>
     </row>
     <row r="2" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="C2" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D2" s="16" t="str">
+        <f>'sign res values'!C2</f>
+        <v>Demand</v>
+      </c>
+      <c r="E2" s="16" t="str">
+        <f>'sign res values'!D2</f>
+        <v xml:space="preserve">Supply </v>
+      </c>
+      <c r="F2" s="16" t="str">
+        <f>'sign res values'!E2</f>
+        <v>Money</v>
+      </c>
       <c r="G2" s="15"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -18988,17 +19076,17 @@
       <c r="I3" s="11"/>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="96" t="s">
         <v>1462</v>
       </c>
       <c r="G4" s="37"/>
@@ -19010,13 +19098,13 @@
       <c r="C5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="96" t="s">
         <v>1462</v>
       </c>
       <c r="G5" s="37"/>
@@ -19024,15 +19112,15 @@
       <c r="I5" s="11"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>1462</v>
       </c>
       <c r="G6" s="37"/>
@@ -19111,7 +19199,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19156,12 +19244,8 @@
       <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="C4" s="92" t="s">
-        <v>1605</v>
-      </c>
-      <c r="D4" s="92" t="s">
-        <v>1604</v>
-      </c>
+      <c r="C4" s="90"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="90"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -19169,6 +19253,15 @@
       <c r="B5" s="15" t="s">
         <v>1332</v>
       </c>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="M5" t="s">
+        <v>1604</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1605</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="88"/>
@@ -19178,12 +19271,12 @@
       <c r="C6" s="90"/>
       <c r="D6" s="90"/>
       <c r="E6" s="90"/>
-      <c r="M6" s="97" t="s">
-        <v>1609</v>
-      </c>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97" t="s">
-        <v>1610</v>
+      <c r="M6" s="98" t="s">
+        <v>1602</v>
+      </c>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98" t="s">
+        <v>1603</v>
       </c>
     </row>
   </sheetData>
@@ -19199,19 +19292,19 @@
   <dimension ref="C1:H6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F4" sqref="F4:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95" t="s">
         <v>1582</v>
       </c>
       <c r="F1" s="16" t="str">
-        <f>'sign res values'!E1</f>
+        <f>'sign res values'!E2</f>
         <v>Money</v>
       </c>
       <c r="G1" s="16">
@@ -19224,16 +19317,16 @@
       </c>
     </row>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
       <c r="E3" s="15"/>
       <c r="F3" s="46" t="s">
         <v>1331</v>
@@ -19246,38 +19339,34 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="F4" s="95" t="s">
-        <v>1462</v>
-      </c>
-      <c r="G4" s="95" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H4" s="95"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
       <c r="E6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19292,35 +19381,35 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="93"/>
-      <c r="B1" s="94" t="s">
+      <c r="A1" s="94"/>
+      <c r="B1" s="95" t="s">
         <v>1582</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="95" t="s">
         <v>1583</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="95" t="s">
         <v>1584</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="95" t="s">
         <v>1585</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="93"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="15"/>
       <c r="C3" s="46" t="s">
         <v>1331</v>
@@ -19333,22 +19422,22 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="C4" s="95"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="95"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
       <c r="O5" t="s">
         <v>1606</v>
       </c>
@@ -19357,13 +19446,13 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
       <c r="O6" t="s">
         <v>1607</v>
       </c>
@@ -19380,42 +19469,42 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="93"/>
-      <c r="B1" s="93"/>
-      <c r="C1" s="94" t="s">
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="95" t="s">
         <v>1582</v>
       </c>
       <c r="D1" s="16" t="str">
-        <f>'sign res values'!C1</f>
+        <f>'sign res values'!C2</f>
         <v>Demand</v>
       </c>
       <c r="E1" s="16" t="str">
-        <f>'sign res values'!D1</f>
+        <f>'sign res values'!D2</f>
         <v xml:space="preserve">Supply </v>
       </c>
       <c r="F1" s="16" t="str">
-        <f>'sign res values'!E1</f>
+        <f>'sign res values'!E2</f>
         <v>Money</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="93"/>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
-      <c r="B3" s="93"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
       <c r="C3" s="15"/>
       <c r="D3" s="46" t="s">
         <v>1331</v>
@@ -19428,34 +19517,44 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
       <c r="C4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
+      <c r="D4" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E4" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>1462</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
-      <c r="B5" s="93"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
       <c r="C5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
+      <c r="D5" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F5" s="96"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="93"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19469,7 +19568,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Removed ans=0 from results file
</commit_message>
<xml_diff>
--- a/tbx/bear/data.xlsx
+++ b/tbx/bear/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7785" tabRatio="946" firstSheet="15" activeTab="25"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7785" tabRatio="946" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="12" r:id="rId1"/>
@@ -44,6 +44,9 @@
     <sheet name="pan blocks" sheetId="47" r:id="rId35"/>
     <sheet name="DSAFO32ADVVERINF32" sheetId="50" state="hidden" r:id="rId36"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId37"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_DLX1.INC" localSheetId="12">#REF!</definedName>
     <definedName name="_DLX1.INC" localSheetId="13">#REF!</definedName>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="1611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="1613">
   <si>
     <t>1999q1</t>
   </si>
@@ -5014,9 +5017,6 @@
     <t>AR prior</t>
   </si>
   <si>
-    <t>0 0.1</t>
-  </si>
-  <si>
     <t>Exogenous variables - tightness</t>
   </si>
   <si>
@@ -5038,9 +5038,6 @@
     <t>Constant</t>
   </si>
   <si>
-    <t>2003q2 2014q4</t>
-  </si>
-  <si>
     <t>transformation</t>
   </si>
   <si>
@@ -5065,6 +5062,12 @@
     <t>S1</t>
   </si>
   <si>
+    <t>Weaker</t>
+  </si>
+  <si>
+    <t>Stronger</t>
+  </si>
+  <si>
     <t>.Absolute</t>
   </si>
   <si>
@@ -5074,10 +5077,16 @@
     <t xml:space="preserve">&gt;50% </t>
   </si>
   <si>
-    <t>Weaker.W1</t>
-  </si>
-  <si>
-    <t>Stronger.S1</t>
+    <t>9 10</t>
+  </si>
+  <si>
+    <t>2008q2 2014q4</t>
+  </si>
+  <si>
+    <t>0 2</t>
+  </si>
+  <si>
+    <t>0 3</t>
   </si>
 </sst>
 </file>
@@ -5101,7 +5110,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -6243,7 +6251,7 @@
     <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6479,6 +6487,9 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6612,6 +6623,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="data"/>
+      <sheetName val="US"/>
+      <sheetName val="EA"/>
+      <sheetName val="UK"/>
+      <sheetName val="yearly"/>
+      <sheetName val="quarterly"/>
+      <sheetName val="monthly"/>
+      <sheetName val="weekly"/>
+      <sheetName val="daily"/>
+      <sheetName val="undated"/>
+      <sheetName val="AR priors"/>
+      <sheetName val="exo mean priors"/>
+      <sheetName val="exo tight priors"/>
+      <sheetName val="mean adj prior"/>
+      <sheetName val="Long run prior"/>
+      <sheetName val="pred exo"/>
+      <sheetName val="grid"/>
+      <sheetName val="block exo"/>
+      <sheetName val="sign res values"/>
+      <sheetName val="sign res periods"/>
+      <sheetName val="conditions"/>
+      <sheetName val="shocks"/>
+      <sheetName val="blocks"/>
+      <sheetName val="intervals"/>
+      <sheetName val="pan pred exo"/>
+      <sheetName val="pan conditions"/>
+      <sheetName val="pan shocks"/>
+      <sheetName val="pan blocks"/>
+      <sheetName val="DSAFO32ADVVERINF32"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>DOM_GDP</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>Constant</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6906,8 +6998,8 @@
   </sheetPr>
   <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7398,7 +7490,7 @@
       </c>
       <c r="G27" s="63"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>1382</v>
       </c>
@@ -7416,7 +7508,7 @@
       </c>
       <c r="G28" s="63"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>1383</v>
       </c>
@@ -7434,7 +7526,7 @@
       </c>
       <c r="G29" s="63"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
         <v>1384</v>
       </c>
@@ -7452,7 +7544,7 @@
       </c>
       <c r="G30" s="63"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
         <v>1385</v>
       </c>
@@ -7470,7 +7562,7 @@
       </c>
       <c r="G31" s="63"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="43" t="s">
         <v>1386</v>
       </c>
@@ -7488,7 +7580,7 @@
       </c>
       <c r="G32" s="63"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="43" t="s">
         <v>1387</v>
       </c>
@@ -7506,7 +7598,7 @@
       </c>
       <c r="G33" s="63"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="43" t="s">
         <v>1388</v>
       </c>
@@ -7524,7 +7616,7 @@
       </c>
       <c r="G34" s="63"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="43" t="s">
         <v>1389</v>
       </c>
@@ -7542,7 +7634,7 @@
       </c>
       <c r="G35" s="63"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>1390</v>
       </c>
@@ -7560,7 +7652,7 @@
       </c>
       <c r="G36" s="63"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
         <v>1391</v>
       </c>
@@ -7578,7 +7670,7 @@
       </c>
       <c r="G37" s="63"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
         <v>1392</v>
       </c>
@@ -7596,7 +7688,7 @@
       </c>
       <c r="G38" s="63"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>1393</v>
       </c>
@@ -7614,7 +7706,7 @@
       </c>
       <c r="G39" s="63"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
         <v>1394</v>
       </c>
@@ -7632,7 +7724,7 @@
       </c>
       <c r="G40" s="63"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>1395</v>
       </c>
@@ -7650,7 +7742,7 @@
       </c>
       <c r="G41" s="63"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>1396</v>
       </c>
@@ -7668,7 +7760,7 @@
       </c>
       <c r="G42" s="63"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
         <v>1397</v>
       </c>
@@ -7686,7 +7778,7 @@
       </c>
       <c r="G43" s="63"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
         <v>1398</v>
       </c>
@@ -7704,7 +7796,7 @@
       </c>
       <c r="G44" s="63"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
         <v>1399</v>
       </c>
@@ -7722,7 +7814,7 @@
       </c>
       <c r="G45" s="63"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="44" t="s">
         <v>1400</v>
       </c>
@@ -7740,7 +7832,7 @@
       </c>
       <c r="G46" s="63"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="44" t="s">
         <v>1401</v>
       </c>
@@ -7758,7 +7850,7 @@
       </c>
       <c r="G47" s="63"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="44" t="s">
         <v>1402</v>
       </c>
@@ -7776,7 +7868,7 @@
       </c>
       <c r="G48" s="63"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="44" t="s">
         <v>1403</v>
       </c>
@@ -7794,7 +7886,7 @@
       </c>
       <c r="G49" s="63"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="44" t="s">
         <v>1404</v>
       </c>
@@ -7812,7 +7904,7 @@
       </c>
       <c r="G50" s="63"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
         <v>1405</v>
       </c>
@@ -7830,7 +7922,7 @@
       </c>
       <c r="G51" s="63"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="44" t="s">
         <v>1406</v>
       </c>
@@ -7848,7 +7940,7 @@
       </c>
       <c r="G52" s="63"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="44" t="s">
         <v>1407</v>
       </c>
@@ -7866,7 +7958,7 @@
       </c>
       <c r="G53" s="63"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="44" t="s">
         <v>1408</v>
       </c>
@@ -7884,7 +7976,7 @@
       </c>
       <c r="G54" s="63"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="44" t="s">
         <v>1409</v>
       </c>
@@ -7902,7 +7994,7 @@
       </c>
       <c r="G55" s="63"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="44" t="s">
         <v>1410</v>
       </c>
@@ -7920,7 +8012,7 @@
       </c>
       <c r="G56" s="63"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="44" t="s">
         <v>1411</v>
       </c>
@@ -7938,7 +8030,7 @@
       </c>
       <c r="G57" s="63"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="44" t="s">
         <v>1412</v>
       </c>
@@ -7956,7 +8048,7 @@
       </c>
       <c r="G58" s="63"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="44" t="s">
         <v>1413</v>
       </c>
@@ -7974,7 +8066,7 @@
       </c>
       <c r="G59" s="63"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="44" t="s">
         <v>1414</v>
       </c>
@@ -7992,7 +8084,7 @@
       </c>
       <c r="G60" s="63"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="44" t="s">
         <v>1415</v>
       </c>
@@ -8010,7 +8102,7 @@
       </c>
       <c r="G61" s="63"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="44" t="s">
         <v>1416</v>
       </c>
@@ -8028,7 +8120,7 @@
       </c>
       <c r="G62" s="63"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="44" t="s">
         <v>1417</v>
       </c>
@@ -8046,7 +8138,7 @@
       </c>
       <c r="G63" s="63"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="44" t="s">
         <v>1418</v>
       </c>
@@ -8064,7 +8156,7 @@
       </c>
       <c r="G64" s="63"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="44" t="s">
         <v>1419</v>
       </c>
@@ -8082,7 +8174,7 @@
       </c>
       <c r="G65" s="63"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="44" t="s">
         <v>1420</v>
       </c>
@@ -8100,7 +8192,7 @@
       </c>
       <c r="G66" s="63"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="44" t="s">
         <v>1421</v>
       </c>
@@ -8118,7 +8210,7 @@
       </c>
       <c r="G67" s="63"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="44" t="s">
         <v>1422</v>
       </c>
@@ -8136,7 +8228,7 @@
       </c>
       <c r="G68" s="63"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="44" t="s">
         <v>1423</v>
       </c>
@@ -8154,7 +8246,7 @@
       </c>
       <c r="G69" s="63"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="44" t="s">
         <v>1424</v>
       </c>
@@ -8172,7 +8264,7 @@
       </c>
       <c r="G70" s="63"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="44" t="s">
         <v>1425</v>
       </c>
@@ -8190,7 +8282,7 @@
       </c>
       <c r="G71" s="63"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="44" t="s">
         <v>1426</v>
       </c>
@@ -8208,7 +8300,7 @@
       </c>
       <c r="G72" s="63"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="44" t="s">
         <v>1427</v>
       </c>
@@ -8226,7 +8318,7 @@
       </c>
       <c r="G73" s="63"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="44" t="s">
         <v>1428</v>
       </c>
@@ -8244,7 +8336,7 @@
       </c>
       <c r="G74" s="63"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="44" t="s">
         <v>1429</v>
       </c>
@@ -8262,7 +8354,7 @@
       </c>
       <c r="G75" s="63"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="44" t="s">
         <v>1430</v>
       </c>
@@ -8280,7 +8372,7 @@
       </c>
       <c r="G76" s="63"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="44" t="s">
         <v>1431</v>
       </c>
@@ -8298,7 +8390,7 @@
       </c>
       <c r="G77" s="63"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="44" t="s">
         <v>1432</v>
       </c>
@@ -8316,7 +8408,7 @@
       </c>
       <c r="G78" s="63"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="44" t="s">
         <v>1433</v>
       </c>
@@ -8334,7 +8426,7 @@
       </c>
       <c r="G79" s="63"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="44" t="s">
         <v>1434</v>
       </c>
@@ -8352,7 +8444,7 @@
       </c>
       <c r="G80" s="63"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="44" t="s">
         <v>1435</v>
       </c>
@@ -8370,7 +8462,7 @@
       </c>
       <c r="G81" s="63"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="44" t="s">
         <v>1436</v>
       </c>
@@ -8388,7 +8480,7 @@
       </c>
       <c r="G82" s="63"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="44" t="s">
         <v>1437</v>
       </c>
@@ -8406,7 +8498,7 @@
       </c>
       <c r="G83" s="63"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="44" t="s">
         <v>1438</v>
       </c>
@@ -8424,7 +8516,7 @@
       </c>
       <c r="G84" s="63"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="44" t="s">
         <v>1439</v>
       </c>
@@ -8442,7 +8534,7 @@
       </c>
       <c r="G85" s="63"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="44" t="s">
         <v>1440</v>
       </c>
@@ -8460,7 +8552,7 @@
       </c>
       <c r="G86" s="63"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="44" t="s">
         <v>1441</v>
       </c>
@@ -8478,7 +8570,7 @@
       </c>
       <c r="G87" s="63"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="44" t="s">
         <v>1442</v>
       </c>
@@ -8496,7 +8588,7 @@
       </c>
       <c r="G88" s="63"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="44" t="s">
         <v>1443</v>
       </c>
@@ -8514,7 +8606,7 @@
       </c>
       <c r="G89" s="63"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90" s="44" t="s">
         <v>1444</v>
       </c>
@@ -8532,7 +8624,7 @@
       </c>
       <c r="G90" s="63"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="44" t="s">
         <v>1445</v>
       </c>
@@ -8550,7 +8642,7 @@
       </c>
       <c r="G91" s="63"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="44" t="s">
         <v>1334</v>
       </c>
@@ -8568,7 +8660,7 @@
       </c>
       <c r="G92" s="63"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="44" t="s">
         <v>1335</v>
       </c>
@@ -8586,7 +8678,7 @@
       </c>
       <c r="G93" s="63"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="44" t="s">
         <v>1336</v>
       </c>
@@ -8604,7 +8696,7 @@
       </c>
       <c r="G94" s="63"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="44" t="s">
         <v>1337</v>
       </c>
@@ -8622,7 +8714,7 @@
       </c>
       <c r="G95" s="63"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96" s="44" t="s">
         <v>1338</v>
       </c>
@@ -8640,7 +8732,7 @@
       </c>
       <c r="G96" s="63"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="44" t="s">
         <v>1339</v>
       </c>
@@ -8658,7 +8750,7 @@
       </c>
       <c r="G97" s="63"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98" s="44" t="s">
         <v>1340</v>
       </c>
@@ -8676,7 +8768,7 @@
       </c>
       <c r="G98" s="63"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="44" t="s">
         <v>1341</v>
       </c>
@@ -8694,7 +8786,7 @@
       </c>
       <c r="G99" s="63"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
         <v>1342</v>
       </c>
@@ -8712,7 +8804,7 @@
       </c>
       <c r="G100" s="63"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
         <v>1343</v>
       </c>
@@ -8730,7 +8822,7 @@
       </c>
       <c r="G101" s="63"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
         <v>0</v>
       </c>
@@ -8748,7 +8840,7 @@
       </c>
       <c r="G102" s="63"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
         <v>1</v>
       </c>
@@ -8766,7 +8858,7 @@
       </c>
       <c r="G103" s="63"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
         <v>2</v>
       </c>
@@ -8784,7 +8876,7 @@
       </c>
       <c r="G104" s="63"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105" s="44" t="s">
         <v>3</v>
       </c>
@@ -8802,7 +8894,7 @@
       </c>
       <c r="G105" s="63"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
         <v>4</v>
       </c>
@@ -8820,7 +8912,7 @@
       </c>
       <c r="G106" s="63"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107" s="44" t="s">
         <v>5</v>
       </c>
@@ -8838,7 +8930,7 @@
       </c>
       <c r="G107" s="63"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="44" t="s">
         <v>6</v>
       </c>
@@ -8856,7 +8948,7 @@
       </c>
       <c r="G108" s="63"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A109" s="44" t="s">
         <v>7</v>
       </c>
@@ -8874,7 +8966,7 @@
       </c>
       <c r="G109" s="63"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="44" t="s">
         <v>8</v>
       </c>
@@ -8892,7 +8984,7 @@
       </c>
       <c r="G110" s="63"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="44" t="s">
         <v>9</v>
       </c>
@@ -8910,7 +9002,7 @@
       </c>
       <c r="G111" s="63"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="44" t="s">
         <v>10</v>
       </c>
@@ -8928,7 +9020,7 @@
       </c>
       <c r="G112" s="63"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="44" t="s">
         <v>11</v>
       </c>
@@ -8946,7 +9038,7 @@
       </c>
       <c r="G113" s="63"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
         <v>12</v>
       </c>
@@ -8964,7 +9056,7 @@
       </c>
       <c r="G114" s="63"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="44" t="s">
         <v>13</v>
       </c>
@@ -8982,7 +9074,7 @@
       </c>
       <c r="G115" s="63"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>14</v>
       </c>
@@ -9000,7 +9092,7 @@
       </c>
       <c r="G116" s="63"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="44" t="s">
         <v>15</v>
       </c>
@@ -9018,7 +9110,7 @@
       </c>
       <c r="G117" s="63"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
         <v>16</v>
       </c>
@@ -9036,7 +9128,7 @@
       </c>
       <c r="G118" s="63"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="44" t="s">
         <v>17</v>
       </c>
@@ -9054,7 +9146,7 @@
       </c>
       <c r="G119" s="63"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="44" t="s">
         <v>18</v>
       </c>
@@ -9072,7 +9164,7 @@
       </c>
       <c r="G120" s="63"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="44" t="s">
         <v>19</v>
       </c>
@@ -9090,7 +9182,7 @@
       </c>
       <c r="G121" s="63"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="44" t="s">
         <v>20</v>
       </c>
@@ -9108,7 +9200,7 @@
       </c>
       <c r="G122" s="63"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="44" t="s">
         <v>21</v>
       </c>
@@ -9126,7 +9218,7 @@
       </c>
       <c r="G123" s="63"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="44" t="s">
         <v>22</v>
       </c>
@@ -9144,7 +9236,7 @@
       </c>
       <c r="G124" s="63"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="44" t="s">
         <v>23</v>
       </c>
@@ -9162,7 +9254,7 @@
       </c>
       <c r="G125" s="63"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="44" t="s">
         <v>24</v>
       </c>
@@ -9180,7 +9272,7 @@
       </c>
       <c r="G126" s="63"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127" s="44" t="s">
         <v>25</v>
       </c>
@@ -9198,7 +9290,7 @@
       </c>
       <c r="G127" s="63"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128" s="44" t="s">
         <v>26</v>
       </c>
@@ -9216,7 +9308,7 @@
       </c>
       <c r="G128" s="63"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="44" t="s">
         <v>27</v>
       </c>
@@ -9234,7 +9326,7 @@
       </c>
       <c r="G129" s="63"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130" s="44" t="s">
         <v>28</v>
       </c>
@@ -9252,7 +9344,7 @@
       </c>
       <c r="G130" s="63"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131" s="44" t="s">
         <v>29</v>
       </c>
@@ -9270,7 +9362,7 @@
       </c>
       <c r="G131" s="63"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132" s="44" t="s">
         <v>30</v>
       </c>
@@ -9288,7 +9380,7 @@
       </c>
       <c r="G132" s="63"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A133" s="44" t="s">
         <v>31</v>
       </c>
@@ -9306,7 +9398,7 @@
       </c>
       <c r="G133" s="63"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134" s="44" t="s">
         <v>32</v>
       </c>
@@ -9324,7 +9416,7 @@
       </c>
       <c r="G134" s="63"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135" s="44" t="s">
         <v>33</v>
       </c>
@@ -9342,7 +9434,7 @@
       </c>
       <c r="G135" s="63"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136" s="44" t="s">
         <v>34</v>
       </c>
@@ -9360,7 +9452,7 @@
       </c>
       <c r="G136" s="63"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A137" s="44" t="s">
         <v>35</v>
       </c>
@@ -9378,7 +9470,7 @@
       </c>
       <c r="G137" s="63"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A138" s="44" t="s">
         <v>36</v>
       </c>
@@ -9396,7 +9488,7 @@
       </c>
       <c r="G138" s="63"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A139" s="44" t="s">
         <v>37</v>
       </c>
@@ -9414,7 +9506,7 @@
       </c>
       <c r="G139" s="63"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A140" s="44" t="s">
         <v>38</v>
       </c>
@@ -9432,7 +9524,7 @@
       </c>
       <c r="G140" s="63"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141" s="44" t="s">
         <v>39</v>
       </c>
@@ -9450,7 +9542,7 @@
       </c>
       <c r="G141" s="63"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142" s="44" t="s">
         <v>40</v>
       </c>
@@ -9468,7 +9560,7 @@
       </c>
       <c r="G142" s="63"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A143" s="44" t="s">
         <v>41</v>
       </c>
@@ -9486,7 +9578,7 @@
       </c>
       <c r="G143" s="63"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A144" s="44" t="s">
         <v>42</v>
       </c>
@@ -9504,7 +9596,7 @@
       </c>
       <c r="G144" s="63"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A145" s="44" t="s">
         <v>43</v>
       </c>
@@ -9522,7 +9614,7 @@
       </c>
       <c r="G145" s="63"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A146" s="44" t="s">
         <v>44</v>
       </c>
@@ -9540,7 +9632,7 @@
       </c>
       <c r="G146" s="63"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A147" s="44" t="s">
         <v>45</v>
       </c>
@@ -9558,7 +9650,7 @@
       </c>
       <c r="G147" s="63"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A148" s="44" t="s">
         <v>46</v>
       </c>
@@ -9576,7 +9668,7 @@
       </c>
       <c r="G148" s="63"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="44" t="s">
         <v>47</v>
       </c>
@@ -9594,7 +9686,7 @@
       </c>
       <c r="G149" s="63"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="44" t="s">
         <v>48</v>
       </c>
@@ -9612,7 +9704,7 @@
       </c>
       <c r="G150" s="63"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="44" t="s">
         <v>49</v>
       </c>
@@ -9630,7 +9722,7 @@
       </c>
       <c r="G151" s="63"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="44" t="s">
         <v>50</v>
       </c>
@@ -9648,7 +9740,7 @@
       </c>
       <c r="G152" s="63"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A153" s="44" t="s">
         <v>51</v>
       </c>
@@ -9666,7 +9758,7 @@
       </c>
       <c r="G153" s="63"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="44" t="s">
         <v>52</v>
       </c>
@@ -9684,7 +9776,7 @@
       </c>
       <c r="G154" s="63"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A155" s="44" t="s">
         <v>53</v>
       </c>
@@ -9702,7 +9794,7 @@
       </c>
       <c r="G155" s="63"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A156" s="44" t="s">
         <v>54</v>
       </c>
@@ -9720,7 +9812,7 @@
       </c>
       <c r="G156" s="63"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A157" s="44" t="s">
         <v>55</v>
       </c>
@@ -9738,7 +9830,7 @@
       </c>
       <c r="G157" s="63"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A158" s="44" t="s">
         <v>56</v>
       </c>
@@ -9756,7 +9848,7 @@
       </c>
       <c r="G158" s="63"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="44" t="s">
         <v>57</v>
       </c>
@@ -9774,7 +9866,7 @@
       </c>
       <c r="G159" s="63"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A160" s="44" t="s">
         <v>58</v>
       </c>
@@ -9792,7 +9884,7 @@
       </c>
       <c r="G160" s="63"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A161" s="44" t="s">
         <v>59</v>
       </c>
@@ -9810,7 +9902,7 @@
       </c>
       <c r="G161" s="63"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A162" s="44" t="s">
         <v>60</v>
       </c>
@@ -9828,7 +9920,7 @@
       </c>
       <c r="G162" s="63"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A163" s="44" t="s">
         <v>61</v>
       </c>
@@ -9846,7 +9938,7 @@
       </c>
       <c r="G163" s="63"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A164" s="44" t="s">
         <v>62</v>
       </c>
@@ -9864,7 +9956,7 @@
       </c>
       <c r="G164" s="63"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A165" s="44" t="s">
         <v>63</v>
       </c>
@@ -9882,44 +9974,44 @@
       </c>
       <c r="G165" s="63"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="44"/>
       <c r="E166" s="2"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="44"/>
       <c r="E167" s="2"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="44"/>
       <c r="E168" s="2"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="44"/>
       <c r="E169" s="2"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="44"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="44"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="44"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="44"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="44"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="44"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="44"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="44"/>
     </row>
   </sheetData>
@@ -12961,60 +13053,60 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
-        <v>1598</v>
+      <c r="A1" s="92" t="s">
+        <v>1596</v>
       </c>
       <c r="B1" s="88">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="D1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="E1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="92" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="92" t="s">
         <v>1599</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B3" s="88" t="s">
         <v>1600</v>
       </c>
-      <c r="C2" t="s">
-        <v>1603</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1603</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="91" t="s">
+      <c r="C3" t="s">
         <v>1601</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1603</v>
-      </c>
       <c r="D3" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="E3" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -13030,7 +13122,7 @@
         <v>1357</v>
       </c>
       <c r="B5" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -13038,7 +13130,7 @@
         <v>1358</v>
       </c>
       <c r="B6" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -13046,7 +13138,7 @@
         <v>1359</v>
       </c>
       <c r="B7" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -13862,7 +13954,7 @@
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13872,10 +13964,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
         <v>1586</v>
       </c>
-      <c r="C2" s="99"/>
+      <c r="C2" s="100"/>
     </row>
     <row r="3" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="75" t="s">
@@ -13936,13 +14028,13 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="100"/>
+      <c r="G2" s="74" t="s">
         <v>1594</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99"/>
-      <c r="G2" s="74" t="s">
-        <v>1595</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -13950,14 +14042,14 @@
         <v>1587</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="D3" s="87" t="s">
         <v>1451</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="74" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -13971,7 +14063,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14023,28 +14115,29 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="100"/>
+      <c r="G2" s="74" t="s">
         <v>1590</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99"/>
-      <c r="G2" s="74" t="s">
-        <v>1591</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="75" t="s">
         <v>1587</v>
       </c>
-      <c r="C3" s="84" t="s">
-        <v>1596</v>
+      <c r="C3" s="84" t="str">
+        <f>'[1]exo mean priors'!C3</f>
+        <v>Constant</v>
       </c>
       <c r="D3" s="85" t="s">
         <v>1451</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="74" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14058,7 +14151,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14099,8 +14192,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14128,55 +14221,55 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
         <v>1331</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>1328</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>1446</v>
+      <c r="C3" s="96" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>1609</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>1597</v>
+        <v>1610</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="42" t="s">
         <v>1332</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="96" t="s">
         <v>1328</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="96" t="s">
         <v>1446</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>1597</v>
+        <v>1610</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
         <v>1333</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="96" t="s">
         <v>1328</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="96" t="s">
         <v>1455</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>1597</v>
+        <v>1610</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>1589</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -14213,7 +14306,7 @@
   <dimension ref="A2:A165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15301,7 +15394,7 @@
   <dimension ref="B1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18765,7 +18858,7 @@
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18775,26 +18868,25 @@
     <col min="9" max="9" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="11" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1583</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>1584</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>1585</v>
-      </c>
+    <row r="1" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="11"/>
       <c r="G1" s="1"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11"/>
+    <row r="2" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1584</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>1585</v>
+      </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -18820,13 +18912,13 @@
       <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="96" t="s">
         <v>1456</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="97" t="s">
         <v>1456</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="96" t="s">
         <v>1456</v>
       </c>
       <c r="F4" s="37"/>
@@ -18838,13 +18930,13 @@
       <c r="B5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="96" t="s">
         <v>1456</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="96" t="s">
         <v>1461</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="96" t="s">
         <v>1456</v>
       </c>
       <c r="F5" s="37"/>
@@ -18856,11 +18948,11 @@
       <c r="B6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="96" t="s">
         <v>1456</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95" t="s">
+      <c r="D6" s="96"/>
+      <c r="E6" s="96" t="s">
         <v>1461</v>
       </c>
       <c r="F6" s="37"/>
@@ -18930,7 +19022,7 @@
   <dimension ref="C1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18941,32 +19033,28 @@
     <col min="10" max="10" width="95.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="11" t="s">
-        <v>1582</v>
-      </c>
-      <c r="D1" s="16" t="str">
-        <f>'sign res values'!C1</f>
-        <v>Demand</v>
-      </c>
-      <c r="E1" s="16" t="str">
-        <f>'sign res values'!D1</f>
-        <v xml:space="preserve">Supply </v>
-      </c>
-      <c r="F1" s="16" t="str">
-        <f>'sign res values'!E1</f>
-        <v>Money</v>
-      </c>
+    <row r="1" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="16"/>
       <c r="H1" s="1"/>
       <c r="I1" s="11"/>
       <c r="J1" s="14"/>
     </row>
     <row r="2" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="C2" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D2" s="16" t="str">
+        <f>'sign res values'!C2</f>
+        <v>Demand</v>
+      </c>
+      <c r="E2" s="16" t="str">
+        <f>'sign res values'!D2</f>
+        <v xml:space="preserve">Supply </v>
+      </c>
+      <c r="F2" s="16" t="str">
+        <f>'sign res values'!E2</f>
+        <v>Money</v>
+      </c>
       <c r="G2" s="15"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -18988,17 +19076,17 @@
       <c r="I3" s="11"/>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="96" t="s">
         <v>1462</v>
       </c>
       <c r="G4" s="37"/>
@@ -19010,13 +19098,13 @@
       <c r="C5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="96" t="s">
         <v>1462</v>
       </c>
       <c r="G5" s="37"/>
@@ -19024,15 +19112,15 @@
       <c r="I5" s="11"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="96" t="s">
         <v>1462</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>1462</v>
       </c>
       <c r="G6" s="37"/>
@@ -19111,7 +19199,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19156,12 +19244,8 @@
       <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="C4" s="92" t="s">
-        <v>1605</v>
-      </c>
-      <c r="D4" s="92" t="s">
-        <v>1604</v>
-      </c>
+      <c r="C4" s="90"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="90"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -19169,6 +19253,15 @@
       <c r="B5" s="15" t="s">
         <v>1332</v>
       </c>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="M5" t="s">
+        <v>1604</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1605</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="88"/>
@@ -19178,12 +19271,12 @@
       <c r="C6" s="90"/>
       <c r="D6" s="90"/>
       <c r="E6" s="90"/>
-      <c r="M6" s="97" t="s">
-        <v>1609</v>
-      </c>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97" t="s">
-        <v>1610</v>
+      <c r="M6" s="98" t="s">
+        <v>1602</v>
+      </c>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98" t="s">
+        <v>1603</v>
       </c>
     </row>
   </sheetData>
@@ -19199,19 +19292,19 @@
   <dimension ref="C1:H6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F4" sqref="F4:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95" t="s">
         <v>1582</v>
       </c>
       <c r="F1" s="16" t="str">
-        <f>'sign res values'!E1</f>
+        <f>'sign res values'!E2</f>
         <v>Money</v>
       </c>
       <c r="G1" s="16">
@@ -19224,16 +19317,16 @@
       </c>
     </row>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
       <c r="E3" s="15"/>
       <c r="F3" s="46" t="s">
         <v>1331</v>
@@ -19246,38 +19339,34 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="F4" s="95" t="s">
-        <v>1462</v>
-      </c>
-      <c r="G4" s="95" t="s">
-        <v>1462</v>
-      </c>
-      <c r="H4" s="95"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
       <c r="E6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19292,35 +19381,35 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="93"/>
-      <c r="B1" s="94" t="s">
+      <c r="A1" s="94"/>
+      <c r="B1" s="95" t="s">
         <v>1582</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="95" t="s">
         <v>1583</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="95" t="s">
         <v>1584</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="95" t="s">
         <v>1585</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="93"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="15"/>
       <c r="C3" s="46" t="s">
         <v>1331</v>
@@ -19333,22 +19422,22 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="C4" s="95"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="95"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
       <c r="O5" t="s">
         <v>1606</v>
       </c>
@@ -19357,13 +19446,13 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
       <c r="O6" t="s">
         <v>1607</v>
       </c>
@@ -19380,42 +19469,42 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="93"/>
-      <c r="B1" s="93"/>
-      <c r="C1" s="94" t="s">
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="95" t="s">
         <v>1582</v>
       </c>
       <c r="D1" s="16" t="str">
-        <f>'sign res values'!C1</f>
+        <f>'sign res values'!C2</f>
         <v>Demand</v>
       </c>
       <c r="E1" s="16" t="str">
-        <f>'sign res values'!D1</f>
+        <f>'sign res values'!D2</f>
         <v xml:space="preserve">Supply </v>
       </c>
       <c r="F1" s="16" t="str">
-        <f>'sign res values'!E1</f>
+        <f>'sign res values'!E2</f>
         <v>Money</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="93"/>
-      <c r="B2" s="93"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
-      <c r="B3" s="93"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
       <c r="C3" s="15"/>
       <c r="D3" s="46" t="s">
         <v>1331</v>
@@ -19428,34 +19517,44 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
-      <c r="B4" s="93"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
       <c r="C4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
+      <c r="D4" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E4" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>1462</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
-      <c r="B5" s="93"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
       <c r="C5" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
+      <c r="D5" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F5" s="96"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="93"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="15" t="s">
         <v>1333</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19469,7 +19568,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>